<commit_message>
finished review of student coding decisions
</commit_message>
<xml_diff>
--- a/data/planning_and_outcomes.xlsx
+++ b/data/planning_and_outcomes.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="179">
   <si>
     <t>project_key</t>
   </si>
@@ -176,9 +176,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>F-test (2x2 ANOVA)</t>
-  </si>
-  <si>
     <t>F(1,46)=7.89</t>
   </si>
   <si>
@@ -425,12 +422,6 @@
     <t>1b</t>
   </si>
   <si>
-    <t>t-test (regression)</t>
-  </si>
-  <si>
-    <t>&lt; .001</t>
-  </si>
-  <si>
     <t>t(199) = 13.07</t>
   </si>
   <si>
@@ -461,9 +452,6 @@
     <t>Gender Bias in Attributing Creativity</t>
   </si>
   <si>
-    <t>Mixed-Model ANOVA</t>
-  </si>
-  <si>
     <t>F(1,78)=75.02,p&lt;.001</t>
   </si>
   <si>
@@ -497,9 +485,6 @@
     <t>How Will I Be Remembered?</t>
   </si>
   <si>
-    <t>F test (regression)</t>
-  </si>
-  <si>
     <t>F(1, 309)=4.08</t>
   </si>
   <si>
@@ -527,9 +512,6 @@
     <t>Capacity for Visual Features in Mental Rotation</t>
   </si>
   <si>
-    <t>F test (ANOVA within subjects)</t>
-  </si>
-  <si>
     <t>F(1,11)=32.04</t>
   </si>
   <si>
@@ -542,6 +524,9 @@
     <t>http://rpubs.com/lampinen/155174</t>
   </si>
   <si>
+    <t>&lt;0.001</t>
+  </si>
+  <si>
     <t>interaction</t>
   </si>
   <si>
@@ -566,10 +551,19 @@
     <t>d = .51</t>
   </si>
   <si>
-    <t>&lt; 0.001</t>
-  </si>
-  <si>
     <t>Conservative</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>power analysis incorrect, DFT x condition interaction is key test</t>
+  </si>
+  <si>
+    <t>effect chosen is more of a manipulation check, individual cue effects (six in all) were the focus of the study, more descriptive</t>
+  </si>
+  <si>
+    <t>chose a main effect but actually the interaction was more theoretically significant, and actually replicated</t>
   </si>
 </sst>
 </file>
@@ -614,14 +608,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -899,16 +894,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO16"/>
+  <dimension ref="A1:AP16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M8" sqref="M8"/>
+      <selection pane="bottomLeft" activeCell="AI12" sqref="AI12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1021,7 +1016,7 @@
         <v>36</v>
       </c>
       <c r="AL1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="AM1" t="s">
         <v>37</v>
@@ -1032,8 +1027,11 @@
       <c r="AO1" t="s">
         <v>39</v>
       </c>
+      <c r="AP1" t="s">
+        <v>175</v>
+      </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -1061,26 +1059,26 @@
       <c r="I2" t="s">
         <v>46</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="4" t="s">
         <v>48</v>
       </c>
       <c r="L2" t="s">
         <v>46</v>
       </c>
       <c r="M2" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="N2">
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="O2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P2" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="Q2">
         <v>48</v>
@@ -1095,7 +1093,7 @@
         <v>0.82</v>
       </c>
       <c r="U2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="V2">
         <v>51</v>
@@ -1125,7 +1123,7 @@
         <v>42441</v>
       </c>
       <c r="AE2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AF2">
         <v>1</v>
@@ -1134,7 +1132,7 @@
         <v>61</v>
       </c>
       <c r="AH2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AI2">
         <v>0.5</v>
@@ -1149,33 +1147,33 @@
         <v>1</v>
       </c>
       <c r="AM2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AN2" t="s">
         <v>54</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AO2" t="s">
         <v>55</v>
       </c>
-      <c r="AO2" t="s">
+    </row>
+    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>57</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>58</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>59</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>60</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>61</v>
-      </c>
-      <c r="F3" t="s">
-        <v>62</v>
       </c>
       <c r="G3">
         <v>4</v>
@@ -1196,16 +1194,16 @@
         <v>48</v>
       </c>
       <c r="M3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="N3">
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="O3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="Q3">
         <v>122</v>
@@ -1220,7 +1218,7 @@
         <v>0.8</v>
       </c>
       <c r="U3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="V3">
         <v>130</v>
@@ -1250,7 +1248,7 @@
         <v>42441</v>
       </c>
       <c r="AE3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AF3">
         <v>1</v>
@@ -1259,7 +1257,7 @@
         <v>128</v>
       </c>
       <c r="AH3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AI3">
         <v>0.5</v>
@@ -1274,33 +1272,33 @@
         <v>1</v>
       </c>
       <c r="AM3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="AN3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO3" t="s">
         <v>55</v>
       </c>
-      <c r="AO3" t="s">
-        <v>56</v>
-      </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" t="s">
         <v>67</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>68</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>69</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>70</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>71</v>
-      </c>
-      <c r="F4" t="s">
-        <v>72</v>
       </c>
       <c r="G4">
         <v>3</v>
@@ -1315,16 +1313,16 @@
         <v>48</v>
       </c>
       <c r="M4" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="N4" t="s">
+        <v>72</v>
+      </c>
+      <c r="O4" t="s">
         <v>73</v>
       </c>
-      <c r="O4" t="s">
-        <v>74</v>
-      </c>
       <c r="P4" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="Q4">
         <v>550</v>
@@ -1339,7 +1337,7 @@
         <v>0.8</v>
       </c>
       <c r="U4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="V4">
         <v>124</v>
@@ -1362,12 +1360,12 @@
       <c r="AB4" s="2">
         <v>42508</v>
       </c>
-      <c r="AC4" s="6"/>
+      <c r="AC4" s="5"/>
       <c r="AD4" s="2">
         <v>42520</v>
       </c>
       <c r="AE4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AF4">
         <v>1</v>
@@ -1376,7 +1374,7 @@
         <v>124</v>
       </c>
       <c r="AH4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AI4">
         <v>0</v>
@@ -1391,36 +1389,36 @@
         <v>1</v>
       </c>
       <c r="AM4" t="s">
+        <v>76</v>
+      </c>
+      <c r="AN4" t="s">
         <v>77</v>
       </c>
-      <c r="AN4" t="s">
+    </row>
+    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>79</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>80</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>81</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>82</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>83</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
         <v>84</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5" t="s">
-        <v>85</v>
       </c>
       <c r="I5" t="s">
         <v>46</v>
@@ -1429,16 +1427,16 @@
         <v>46</v>
       </c>
       <c r="M5" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="N5" t="s">
+        <v>85</v>
+      </c>
+      <c r="O5" t="s">
         <v>86</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>87</v>
-      </c>
-      <c r="P5" t="s">
-        <v>88</v>
       </c>
       <c r="Q5">
         <v>18</v>
@@ -1453,7 +1451,7 @@
         <v>0.95499999999999996</v>
       </c>
       <c r="U5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="V5">
         <v>19</v>
@@ -1483,16 +1481,16 @@
         <v>42445</v>
       </c>
       <c r="AE5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AF5">
         <v>1</v>
       </c>
-      <c r="AG5" s="4">
+      <c r="AG5" s="3">
         <v>19</v>
       </c>
       <c r="AH5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AI5">
         <v>0.5</v>
@@ -1507,30 +1505,30 @@
         <v>1</v>
       </c>
       <c r="AM5" t="s">
+        <v>89</v>
+      </c>
+      <c r="AN5" t="s">
         <v>90</v>
       </c>
-      <c r="AN5" t="s">
-        <v>91</v>
-      </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" t="s">
         <v>93</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>94</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>95</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>96</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>97</v>
-      </c>
-      <c r="F6" t="s">
-        <v>98</v>
       </c>
       <c r="G6">
         <v>2</v>
@@ -1551,16 +1549,16 @@
         <v>46</v>
       </c>
       <c r="M6" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="N6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="P6" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="Q6">
         <v>219</v>
@@ -1575,7 +1573,7 @@
         <v>0.8</v>
       </c>
       <c r="U6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="V6">
         <v>415</v>
@@ -1605,7 +1603,7 @@
         <v>42445</v>
       </c>
       <c r="AE6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AF6">
         <v>1</v>
@@ -1614,7 +1612,7 @@
         <v>397</v>
       </c>
       <c r="AH6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AI6">
         <v>0</v>
@@ -1629,30 +1627,30 @@
         <v>1</v>
       </c>
       <c r="AM6" t="s">
+        <v>101</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>102</v>
       </c>
-      <c r="AN6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>103</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>104</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>105</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>106</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>107</v>
-      </c>
-      <c r="F7" t="s">
-        <v>108</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -1667,16 +1665,16 @@
         <v>46</v>
       </c>
       <c r="M7" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="N7" t="s">
-        <v>179</v>
-      </c>
-      <c r="O7" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="P7" s="4" t="s">
         <v>109</v>
-      </c>
-      <c r="P7" s="5" t="s">
-        <v>110</v>
       </c>
       <c r="Q7">
         <v>48</v>
@@ -1684,14 +1682,14 @@
       <c r="R7">
         <v>90</v>
       </c>
-      <c r="S7" s="5">
+      <c r="S7" s="4">
         <v>0.57599999999999996</v>
       </c>
       <c r="T7">
         <v>0.8</v>
       </c>
-      <c r="U7" s="5" t="s">
-        <v>180</v>
+      <c r="U7" s="4" t="s">
+        <v>174</v>
       </c>
       <c r="V7">
         <v>95</v>
@@ -1721,7 +1719,7 @@
         <v>42437</v>
       </c>
       <c r="AE7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AF7">
         <v>1</v>
@@ -1730,7 +1728,7 @@
         <v>95</v>
       </c>
       <c r="AH7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AI7">
         <v>0.5</v>
@@ -1741,40 +1739,43 @@
       <c r="AK7">
         <v>4</v>
       </c>
-      <c r="AL7" s="5">
+      <c r="AL7" s="4">
         <v>0</v>
       </c>
       <c r="AM7" t="s">
+        <v>111</v>
+      </c>
+      <c r="AN7" t="s">
         <v>112</v>
       </c>
-      <c r="AN7" t="s">
+      <c r="AP7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>114</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>115</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>116</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>117</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>118</v>
-      </c>
-      <c r="F8" t="s">
-        <v>119</v>
       </c>
       <c r="G8">
         <v>2</v>
       </c>
       <c r="H8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I8" t="s">
         <v>48</v>
@@ -1789,16 +1790,16 @@
         <v>46</v>
       </c>
       <c r="M8" t="s">
-        <v>49</v>
+        <v>169</v>
       </c>
       <c r="N8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="O8" t="s">
+        <v>119</v>
+      </c>
+      <c r="P8" t="s">
         <v>120</v>
-      </c>
-      <c r="P8" t="s">
-        <v>121</v>
       </c>
       <c r="Q8">
         <v>40</v>
@@ -1813,7 +1814,7 @@
         <v>0.95</v>
       </c>
       <c r="U8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="V8">
         <v>42</v>
@@ -1843,7 +1844,7 @@
         <v>42441</v>
       </c>
       <c r="AE8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AF8">
         <v>1</v>
@@ -1852,7 +1853,7 @@
         <v>40</v>
       </c>
       <c r="AH8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AI8">
         <v>1</v>
@@ -1863,34 +1864,40 @@
       <c r="AK8">
         <v>4</v>
       </c>
+      <c r="AL8" s="4">
+        <v>0</v>
+      </c>
       <c r="AM8" t="s">
+        <v>123</v>
+      </c>
+      <c r="AN8" t="s">
+        <v>77</v>
+      </c>
+      <c r="AP8" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="9" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>124</v>
       </c>
-      <c r="AN8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
         <v>125</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>126</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>127</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>128</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>129</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>130</v>
-      </c>
-      <c r="G9" t="s">
-        <v>131</v>
       </c>
       <c r="H9" t="s">
         <v>48</v>
@@ -1902,16 +1909,16 @@
         <v>48</v>
       </c>
       <c r="M9" t="s">
+        <v>169</v>
+      </c>
+      <c r="N9" t="s">
+        <v>85</v>
+      </c>
+      <c r="O9" t="s">
+        <v>131</v>
+      </c>
+      <c r="P9" t="s">
         <v>132</v>
-      </c>
-      <c r="N9" t="s">
-        <v>133</v>
-      </c>
-      <c r="O9" t="s">
-        <v>134</v>
-      </c>
-      <c r="P9" t="s">
-        <v>135</v>
       </c>
       <c r="Q9">
         <v>202</v>
@@ -1926,7 +1933,7 @@
         <v>0.93089999999999995</v>
       </c>
       <c r="U9" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="V9">
         <v>53</v>
@@ -1956,7 +1963,7 @@
         <v>42437</v>
       </c>
       <c r="AE9" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AF9">
         <v>1</v>
@@ -1965,7 +1972,7 @@
         <v>50</v>
       </c>
       <c r="AH9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AI9">
         <v>1</v>
@@ -1976,31 +1983,34 @@
       <c r="AK9">
         <v>6</v>
       </c>
+      <c r="AL9">
+        <v>1</v>
+      </c>
       <c r="AM9" t="s">
+        <v>134</v>
+      </c>
+      <c r="AN9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10" t="s">
+        <v>136</v>
+      </c>
+      <c r="C10" t="s">
         <v>137</v>
       </c>
-      <c r="AN9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="D10" t="s">
         <v>138</v>
       </c>
-      <c r="B10" t="s">
+      <c r="E10" t="s">
         <v>139</v>
       </c>
-      <c r="C10" t="s">
+      <c r="F10" t="s">
         <v>140</v>
-      </c>
-      <c r="D10" t="s">
-        <v>141</v>
-      </c>
-      <c r="E10" t="s">
-        <v>142</v>
-      </c>
-      <c r="F10" t="s">
-        <v>143</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -2014,23 +2024,23 @@
       <c r="J10" s="2">
         <v>42775</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="K10" s="4" t="s">
         <v>48</v>
       </c>
       <c r="L10" t="s">
         <v>48</v>
       </c>
-      <c r="M10" t="s">
-        <v>144</v>
+      <c r="M10" s="4" t="s">
+        <v>169</v>
       </c>
       <c r="N10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="O10" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="P10" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="Q10">
         <v>80</v>
@@ -2045,7 +2055,7 @@
         <v>0.8</v>
       </c>
       <c r="U10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="V10">
         <v>84</v>
@@ -2075,7 +2085,7 @@
         <v>42437</v>
       </c>
       <c r="AE10" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="AF10">
         <v>1</v>
@@ -2084,7 +2094,7 @@
         <v>84</v>
       </c>
       <c r="AH10" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="AI10">
         <v>1</v>
@@ -2095,31 +2105,37 @@
       <c r="AK10">
         <v>6.5</v>
       </c>
+      <c r="AL10" s="4">
+        <v>0</v>
+      </c>
       <c r="AM10" t="s">
+        <v>145</v>
+      </c>
+      <c r="AN10" t="s">
+        <v>112</v>
+      </c>
+      <c r="AP10" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="11" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>146</v>
+      </c>
+      <c r="B11" t="s">
+        <v>147</v>
+      </c>
+      <c r="C11" t="s">
+        <v>148</v>
+      </c>
+      <c r="D11" t="s">
         <v>149</v>
       </c>
-      <c r="AN10" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="E11" t="s">
         <v>150</v>
       </c>
-      <c r="B11" t="s">
+      <c r="F11" t="s">
         <v>151</v>
-      </c>
-      <c r="C11" t="s">
-        <v>152</v>
-      </c>
-      <c r="D11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E11" t="s">
-        <v>154</v>
-      </c>
-      <c r="F11" t="s">
-        <v>155</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -2134,13 +2150,13 @@
         <v>48</v>
       </c>
       <c r="M11" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="N11">
         <v>0.04</v>
       </c>
       <c r="O11" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="P11">
         <v>0.36</v>
@@ -2158,13 +2174,13 @@
         <v>0.88</v>
       </c>
       <c r="U11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="V11">
         <v>328</v>
       </c>
       <c r="W11" s="3">
-        <v>42406</v>
+        <v>4</v>
       </c>
       <c r="X11" s="1">
         <v>0.4</v>
@@ -2188,7 +2204,7 @@
         <v>42438</v>
       </c>
       <c r="AE11" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="AF11">
         <v>1</v>
@@ -2197,7 +2213,7 @@
         <v>328</v>
       </c>
       <c r="AH11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AI11">
         <v>0.5</v>
@@ -2208,34 +2224,37 @@
       <c r="AK11">
         <v>4.5</v>
       </c>
+      <c r="AL11" s="6">
+        <v>1</v>
+      </c>
       <c r="AM11" t="s">
+        <v>154</v>
+      </c>
+      <c r="AN11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>155</v>
+      </c>
+      <c r="B12" t="s">
+        <v>156</v>
+      </c>
+      <c r="C12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D12" t="s">
+        <v>158</v>
+      </c>
+      <c r="E12" t="s">
         <v>159</v>
       </c>
-      <c r="AN11" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="F12" t="s">
         <v>160</v>
       </c>
-      <c r="B12" t="s">
-        <v>161</v>
-      </c>
-      <c r="C12" t="s">
-        <v>162</v>
-      </c>
-      <c r="D12" t="s">
-        <v>163</v>
-      </c>
-      <c r="E12" t="s">
-        <v>164</v>
-      </c>
-      <c r="F12" t="s">
-        <v>165</v>
-      </c>
       <c r="G12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H12" t="s">
         <v>46</v>
@@ -2253,16 +2272,16 @@
         <v>46</v>
       </c>
       <c r="M12" t="s">
-        <v>166</v>
-      </c>
-      <c r="N12">
-        <v>1E-3</v>
+        <v>169</v>
+      </c>
+      <c r="N12" t="s">
+        <v>165</v>
       </c>
       <c r="O12" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="P12" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="Q12">
         <v>12</v>
@@ -2277,7 +2296,7 @@
         <v>0.92</v>
       </c>
       <c r="U12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="V12">
         <v>13</v>
@@ -2307,7 +2326,7 @@
         <v>42438</v>
       </c>
       <c r="AE12" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="AF12">
         <v>1</v>
@@ -2316,7 +2335,7 @@
         <v>27</v>
       </c>
       <c r="AH12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AI12">
         <v>0.5</v>
@@ -2327,14 +2346,17 @@
       <c r="AK12">
         <v>4</v>
       </c>
+      <c r="AL12" s="7">
+        <v>1</v>
+      </c>
       <c r="AM12" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AN12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.2">
       <c r="X16" s="1"/>
       <c r="Y16" s="1"/>
       <c r="Z16" s="2"/>

</xml_diff>

<commit_message>
Extracted t stat and ef from original
</commit_message>
<xml_diff>
--- a/data/planning_and_outcomes.xlsx
+++ b/data/planning_and_outcomes.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27224"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcfrank/Projects/replication254/replication_project/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25516"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="460" windowWidth="26340" windowHeight="16360" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="planning_and_outcomes" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="185">
   <si>
     <t>project_key</t>
   </si>
@@ -570,6 +565,18 @@
   </si>
   <si>
     <t>Conservative</t>
+  </si>
+  <si>
+    <t>d=0.36</t>
+  </si>
+  <si>
+    <t>original_t_stat</t>
+  </si>
+  <si>
+    <t>original_t_df</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -577,7 +584,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -616,7 +623,7 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -679,7 +686,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -714,7 +721,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -891,7 +898,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -899,16 +906,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO16"/>
+  <dimension ref="A1:AQ16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M8" sqref="M8"/>
+      <selection pane="bottomLeft" activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="17" max="17" width="18.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:43">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -952,88 +962,94 @@
         <v>13</v>
       </c>
       <c r="O1" t="s">
+        <v>182</v>
+      </c>
+      <c r="P1" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AH1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AI1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AJ1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AK1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AL1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AM1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AN1" t="s">
         <v>172</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AO1" t="s">
         <v>37</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AP1" t="s">
         <v>38</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AQ1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:43">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -1076,89 +1092,96 @@
       <c r="N2">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2">
+        <f>SQRT(7.89)</f>
+        <v>2.8089143810376278</v>
+      </c>
+      <c r="P2">
+        <v>46</v>
+      </c>
+      <c r="Q2" t="s">
         <v>50</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>176</v>
       </c>
-      <c r="Q2">
+      <c r="S2">
         <v>48</v>
       </c>
-      <c r="R2">
+      <c r="T2">
         <v>48</v>
       </c>
-      <c r="S2">
+      <c r="U2">
         <v>0.82</v>
       </c>
-      <c r="T2">
+      <c r="V2">
         <v>0.82</v>
       </c>
-      <c r="U2" t="s">
+      <c r="W2" t="s">
         <v>51</v>
       </c>
-      <c r="V2">
+      <c r="X2">
         <v>51</v>
       </c>
-      <c r="W2">
+      <c r="Y2">
         <v>22</v>
       </c>
-      <c r="X2" s="1">
+      <c r="Z2" s="1">
         <v>2.2000000000000002</v>
       </c>
-      <c r="Y2" s="1">
+      <c r="AA2" s="1">
         <v>147.84</v>
       </c>
-      <c r="Z2" s="2">
+      <c r="AB2" s="2">
         <v>42434</v>
       </c>
-      <c r="AA2" s="2">
+      <c r="AC2" s="2">
         <v>42438</v>
       </c>
-      <c r="AB2" s="2">
+      <c r="AD2" s="2">
         <v>42440</v>
       </c>
-      <c r="AC2" s="2">
+      <c r="AE2" s="2">
         <v>42441</v>
       </c>
-      <c r="AD2" s="2">
+      <c r="AF2" s="2">
         <v>42441</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AG2" t="s">
         <v>52</v>
       </c>
-      <c r="AF2">
-        <v>1</v>
-      </c>
-      <c r="AG2">
+      <c r="AH2">
+        <v>1</v>
+      </c>
+      <c r="AI2">
         <v>61</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AJ2" t="s">
         <v>53</v>
       </c>
-      <c r="AI2">
+      <c r="AK2">
         <v>0.5</v>
       </c>
-      <c r="AJ2">
+      <c r="AL2">
         <v>0.5</v>
       </c>
-      <c r="AK2">
+      <c r="AM2">
         <v>4</v>
       </c>
-      <c r="AL2">
-        <v>1</v>
-      </c>
-      <c r="AM2" t="s">
+      <c r="AN2">
+        <v>1</v>
+      </c>
+      <c r="AO2" t="s">
         <v>54</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AP2" t="s">
         <v>55</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AQ2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:43">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -1201,89 +1224,96 @@
       <c r="N3">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3">
+        <f>SQRT(7.497)</f>
+        <v>2.7380650101851125</v>
+      </c>
+      <c r="P3">
+        <v>115</v>
+      </c>
+      <c r="Q3" t="s">
         <v>63</v>
       </c>
-      <c r="P3" t="s">
+      <c r="R3" t="s">
         <v>178</v>
       </c>
-      <c r="Q3">
+      <c r="S3">
         <v>122</v>
       </c>
-      <c r="R3">
+      <c r="T3">
         <v>123</v>
       </c>
-      <c r="S3">
+      <c r="U3">
         <v>0.8</v>
       </c>
-      <c r="T3">
+      <c r="V3">
         <v>0.8</v>
       </c>
-      <c r="U3" t="s">
+      <c r="W3" t="s">
         <v>64</v>
       </c>
-      <c r="V3">
+      <c r="X3">
         <v>130</v>
       </c>
-      <c r="W3">
+      <c r="Y3">
         <v>3</v>
       </c>
-      <c r="X3" s="1">
+      <c r="Z3" s="1">
         <v>0.3</v>
       </c>
-      <c r="Y3" s="1">
+      <c r="AA3" s="1">
         <v>44.28</v>
       </c>
-      <c r="Z3" s="2">
+      <c r="AB3" s="2">
         <v>42420</v>
       </c>
-      <c r="AA3" s="2">
+      <c r="AC3" s="2">
         <v>42434</v>
       </c>
-      <c r="AB3" s="2">
+      <c r="AD3" s="2">
         <v>42438</v>
       </c>
-      <c r="AC3" s="2">
+      <c r="AE3" s="2">
         <v>42441</v>
       </c>
-      <c r="AD3" s="2">
+      <c r="AF3" s="2">
         <v>42441</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AG3" t="s">
         <v>65</v>
       </c>
-      <c r="AF3">
-        <v>1</v>
-      </c>
-      <c r="AG3">
+      <c r="AH3">
+        <v>1</v>
+      </c>
+      <c r="AI3">
         <v>128</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="AJ3" t="s">
         <v>66</v>
       </c>
-      <c r="AI3">
+      <c r="AK3">
         <v>0.5</v>
       </c>
-      <c r="AJ3">
+      <c r="AL3">
         <v>0.5</v>
       </c>
-      <c r="AK3">
+      <c r="AM3">
         <v>6.5</v>
       </c>
-      <c r="AL3">
-        <v>1</v>
-      </c>
-      <c r="AM3" t="s">
+      <c r="AN3">
+        <v>1</v>
+      </c>
+      <c r="AO3" t="s">
         <v>173</v>
       </c>
-      <c r="AN3" t="s">
+      <c r="AP3" t="s">
         <v>55</v>
       </c>
-      <c r="AO3" t="s">
+      <c r="AQ3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:43">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -1320,84 +1350,91 @@
       <c r="N4" t="s">
         <v>73</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4">
+        <f>2.42</f>
+        <v>2.42</v>
+      </c>
+      <c r="P4">
+        <v>257</v>
+      </c>
+      <c r="Q4" t="s">
         <v>74</v>
       </c>
-      <c r="P4" t="s">
+      <c r="R4" t="s">
         <v>177</v>
       </c>
-      <c r="Q4">
+      <c r="S4">
         <v>550</v>
       </c>
-      <c r="R4">
+      <c r="T4">
         <v>116</v>
       </c>
-      <c r="S4">
+      <c r="U4">
         <v>0.67500000000000004</v>
       </c>
-      <c r="T4">
+      <c r="V4">
         <v>0.8</v>
       </c>
-      <c r="U4" t="s">
+      <c r="W4" t="s">
         <v>64</v>
       </c>
-      <c r="V4">
+      <c r="X4">
         <v>124</v>
       </c>
-      <c r="W4">
+      <c r="Y4">
         <v>10</v>
       </c>
-      <c r="X4" s="1">
+      <c r="Z4" s="1">
         <v>1.1399999999999999</v>
       </c>
-      <c r="Y4" s="1">
+      <c r="AA4" s="1">
         <v>185.14</v>
       </c>
-      <c r="Z4" s="2">
+      <c r="AB4" s="2">
         <v>42456</v>
       </c>
-      <c r="AA4" s="2">
+      <c r="AC4" s="2">
         <v>42477</v>
       </c>
-      <c r="AB4" s="2">
+      <c r="AD4" s="2">
         <v>42508</v>
       </c>
-      <c r="AC4" s="6"/>
-      <c r="AD4" s="2">
+      <c r="AE4" s="6"/>
+      <c r="AF4" s="2">
         <v>42520</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AG4" t="s">
         <v>75</v>
       </c>
-      <c r="AF4">
-        <v>1</v>
-      </c>
-      <c r="AG4">
+      <c r="AH4">
+        <v>1</v>
+      </c>
+      <c r="AI4">
         <v>124</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AJ4" t="s">
         <v>76</v>
       </c>
-      <c r="AI4">
+      <c r="AK4">
         <v>0</v>
       </c>
-      <c r="AJ4">
+      <c r="AL4">
         <v>0</v>
       </c>
-      <c r="AK4">
+      <c r="AM4">
         <v>3.5</v>
       </c>
-      <c r="AL4">
-        <v>1</v>
-      </c>
-      <c r="AM4" t="s">
+      <c r="AN4">
+        <v>1</v>
+      </c>
+      <c r="AO4" t="s">
         <v>77</v>
       </c>
-      <c r="AN4" t="s">
+      <c r="AP4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:43">
       <c r="A5" t="s">
         <v>79</v>
       </c>
@@ -1434,86 +1471,92 @@
       <c r="N5" t="s">
         <v>86</v>
       </c>
-      <c r="O5" t="s">
+      <c r="O5">
+        <v>5.22</v>
+      </c>
+      <c r="P5">
+        <v>17</v>
+      </c>
+      <c r="Q5" t="s">
         <v>87</v>
       </c>
-      <c r="P5" t="s">
+      <c r="R5" t="s">
         <v>88</v>
       </c>
-      <c r="Q5">
+      <c r="S5">
         <v>18</v>
       </c>
-      <c r="R5">
+      <c r="T5">
         <v>18</v>
       </c>
-      <c r="S5">
+      <c r="U5">
         <v>0.92</v>
       </c>
-      <c r="T5">
+      <c r="V5">
         <v>0.95499999999999996</v>
       </c>
-      <c r="U5" t="s">
+      <c r="W5" t="s">
         <v>51</v>
       </c>
-      <c r="V5">
+      <c r="X5">
         <v>19</v>
       </c>
-      <c r="W5">
+      <c r="Y5">
         <v>35</v>
       </c>
-      <c r="X5" s="1">
+      <c r="Z5" s="1">
         <v>3</v>
       </c>
-      <c r="Y5" s="1">
+      <c r="AA5" s="1">
         <v>79.8</v>
       </c>
-      <c r="Z5" s="2">
+      <c r="AB5" s="2">
         <v>42436</v>
       </c>
-      <c r="AA5" s="2">
+      <c r="AC5" s="2">
         <v>42438</v>
-      </c>
-      <c r="AB5" s="2">
-        <v>42445</v>
-      </c>
-      <c r="AC5" s="2">
-        <v>42445</v>
       </c>
       <c r="AD5" s="2">
         <v>42445</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AE5" s="2">
+        <v>42445</v>
+      </c>
+      <c r="AF5" s="2">
+        <v>42445</v>
+      </c>
+      <c r="AG5" t="s">
         <v>89</v>
       </c>
-      <c r="AF5">
-        <v>1</v>
-      </c>
-      <c r="AG5" s="4">
+      <c r="AH5">
+        <v>1</v>
+      </c>
+      <c r="AI5" s="4">
         <v>19</v>
       </c>
-      <c r="AH5" t="s">
+      <c r="AJ5" t="s">
         <v>53</v>
       </c>
-      <c r="AI5">
+      <c r="AK5">
         <v>0.5</v>
       </c>
-      <c r="AJ5">
+      <c r="AL5">
         <v>0.5</v>
       </c>
-      <c r="AK5">
+      <c r="AM5">
         <v>4.5</v>
       </c>
-      <c r="AL5">
-        <v>1</v>
-      </c>
-      <c r="AM5" t="s">
+      <c r="AN5">
+        <v>1</v>
+      </c>
+      <c r="AO5" t="s">
         <v>90</v>
       </c>
-      <c r="AN5" t="s">
+      <c r="AP5" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:43">
       <c r="A6" t="s">
         <v>93</v>
       </c>
@@ -1556,86 +1599,93 @@
       <c r="N6" t="s">
         <v>73</v>
       </c>
-      <c r="O6" t="s">
+      <c r="O6">
+        <f>SQRT(5.18)</f>
+        <v>2.2759613353482084</v>
+      </c>
+      <c r="P6">
+        <v>209</v>
+      </c>
+      <c r="Q6" t="s">
         <v>99</v>
       </c>
-      <c r="P6" t="s">
+      <c r="R6" t="s">
         <v>175</v>
       </c>
-      <c r="Q6">
+      <c r="S6">
         <v>219</v>
       </c>
-      <c r="R6">
+      <c r="T6">
         <v>395</v>
       </c>
-      <c r="S6">
+      <c r="U6">
         <v>0.55000000000000004</v>
       </c>
-      <c r="T6">
+      <c r="V6">
         <v>0.8</v>
       </c>
-      <c r="U6" t="s">
+      <c r="W6" t="s">
         <v>64</v>
       </c>
-      <c r="V6">
+      <c r="X6">
         <v>415</v>
       </c>
-      <c r="W6">
+      <c r="Y6">
         <v>8</v>
       </c>
-      <c r="X6" s="1">
+      <c r="Z6" s="1">
         <v>0.8</v>
       </c>
-      <c r="Y6" s="1">
+      <c r="AA6" s="1">
         <v>442.4</v>
       </c>
-      <c r="Z6" s="2">
+      <c r="AB6" s="2">
         <v>42438</v>
       </c>
-      <c r="AA6" s="2">
+      <c r="AC6" s="2">
         <v>42440</v>
       </c>
-      <c r="AB6" s="2">
+      <c r="AD6" s="2">
         <v>42443</v>
       </c>
-      <c r="AC6" s="2">
+      <c r="AE6" s="2">
         <v>42445</v>
       </c>
-      <c r="AD6" s="2">
+      <c r="AF6" s="2">
         <v>42445</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AG6" t="s">
         <v>100</v>
       </c>
-      <c r="AF6">
-        <v>1</v>
-      </c>
-      <c r="AG6">
+      <c r="AH6">
+        <v>1</v>
+      </c>
+      <c r="AI6">
         <v>397</v>
       </c>
-      <c r="AH6" t="s">
+      <c r="AJ6" t="s">
         <v>101</v>
       </c>
-      <c r="AI6">
+      <c r="AK6">
         <v>0</v>
       </c>
-      <c r="AJ6">
+      <c r="AL6">
         <v>0</v>
       </c>
-      <c r="AK6">
+      <c r="AM6">
         <v>4</v>
       </c>
-      <c r="AL6">
-        <v>1</v>
-      </c>
-      <c r="AM6" t="s">
+      <c r="AN6">
+        <v>1</v>
+      </c>
+      <c r="AO6" t="s">
         <v>102</v>
       </c>
-      <c r="AN6" t="s">
+      <c r="AP6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:43">
       <c r="A7" t="s">
         <v>103</v>
       </c>
@@ -1672,86 +1722,92 @@
       <c r="N7" t="s">
         <v>179</v>
       </c>
-      <c r="O7" s="5" t="s">
+      <c r="O7" t="s">
+        <v>184</v>
+      </c>
+      <c r="P7" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q7" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="P7" s="5" t="s">
+      <c r="R7" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="Q7">
+      <c r="S7">
         <v>48</v>
       </c>
-      <c r="R7">
+      <c r="T7">
         <v>90</v>
       </c>
-      <c r="S7" s="5">
+      <c r="U7" s="5">
         <v>0.57599999999999996</v>
       </c>
-      <c r="T7">
+      <c r="V7">
         <v>0.8</v>
       </c>
-      <c r="U7" s="5" t="s">
+      <c r="W7" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="V7">
+      <c r="X7">
         <v>95</v>
       </c>
-      <c r="W7">
+      <c r="Y7">
         <v>3</v>
       </c>
-      <c r="X7" s="1">
+      <c r="Z7" s="1">
         <v>0.3</v>
       </c>
-      <c r="Y7" s="1">
+      <c r="AA7" s="1">
         <v>37.799999999999997</v>
       </c>
-      <c r="Z7" s="2">
+      <c r="AB7" s="2">
         <v>42419</v>
       </c>
-      <c r="AA7" s="2">
+      <c r="AC7" s="2">
         <v>42435</v>
       </c>
-      <c r="AB7" s="2">
+      <c r="AD7" s="2">
         <v>42436</v>
       </c>
-      <c r="AC7" s="2">
+      <c r="AE7" s="2">
         <v>42437</v>
       </c>
-      <c r="AD7" s="2">
+      <c r="AF7" s="2">
         <v>42437</v>
       </c>
-      <c r="AE7" t="s">
+      <c r="AG7" t="s">
         <v>111</v>
       </c>
-      <c r="AF7">
-        <v>1</v>
-      </c>
-      <c r="AG7">
+      <c r="AH7">
+        <v>1</v>
+      </c>
+      <c r="AI7">
         <v>95</v>
       </c>
-      <c r="AH7" t="s">
+      <c r="AJ7" t="s">
         <v>76</v>
       </c>
-      <c r="AI7">
+      <c r="AK7">
         <v>0.5</v>
       </c>
-      <c r="AJ7">
+      <c r="AL7">
         <v>0.5</v>
       </c>
-      <c r="AK7">
+      <c r="AM7">
         <v>4</v>
       </c>
-      <c r="AL7" s="5">
+      <c r="AN7" s="5">
         <v>0</v>
       </c>
-      <c r="AM7" t="s">
+      <c r="AO7" t="s">
         <v>112</v>
       </c>
-      <c r="AN7" t="s">
+      <c r="AP7" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:43">
       <c r="A8" t="s">
         <v>114</v>
       </c>
@@ -1794,83 +1850,90 @@
       <c r="N8" t="s">
         <v>86</v>
       </c>
-      <c r="O8" t="s">
+      <c r="O8">
+        <f>SQRT(83.67)</f>
+        <v>9.1471306976559603</v>
+      </c>
+      <c r="P8">
+        <v>55</v>
+      </c>
+      <c r="Q8" t="s">
         <v>120</v>
       </c>
-      <c r="P8" t="s">
+      <c r="R8" t="s">
         <v>121</v>
       </c>
-      <c r="Q8">
+      <c r="S8">
         <v>40</v>
       </c>
-      <c r="R8">
+      <c r="T8">
         <v>40</v>
       </c>
-      <c r="S8">
+      <c r="U8">
         <v>0.999</v>
       </c>
-      <c r="T8">
+      <c r="V8">
         <v>0.95</v>
       </c>
-      <c r="U8" t="s">
+      <c r="W8" t="s">
         <v>51</v>
       </c>
-      <c r="V8">
+      <c r="X8">
         <v>42</v>
       </c>
-      <c r="W8">
+      <c r="Y8">
         <v>20</v>
       </c>
-      <c r="X8" s="1">
+      <c r="Z8" s="1">
         <v>2</v>
       </c>
-      <c r="Y8" s="1">
+      <c r="AA8" s="1">
         <v>112</v>
       </c>
-      <c r="Z8" s="2">
+      <c r="AB8" s="2">
         <v>42437</v>
       </c>
-      <c r="AA8" s="2">
+      <c r="AC8" s="2">
         <v>42437</v>
       </c>
-      <c r="AB8" s="2">
+      <c r="AD8" s="2">
         <v>42440</v>
       </c>
-      <c r="AC8" s="2">
+      <c r="AE8" s="2">
         <v>42441</v>
       </c>
-      <c r="AD8" s="2">
+      <c r="AF8" s="2">
         <v>42441</v>
       </c>
-      <c r="AE8" t="s">
+      <c r="AG8" t="s">
         <v>122</v>
       </c>
-      <c r="AF8">
-        <v>1</v>
-      </c>
-      <c r="AG8">
+      <c r="AH8">
+        <v>1</v>
+      </c>
+      <c r="AI8">
         <v>40</v>
       </c>
-      <c r="AH8" t="s">
+      <c r="AJ8" t="s">
         <v>123</v>
       </c>
-      <c r="AI8">
-        <v>1</v>
-      </c>
-      <c r="AJ8">
-        <v>1</v>
-      </c>
       <c r="AK8">
+        <v>1</v>
+      </c>
+      <c r="AL8">
+        <v>1</v>
+      </c>
+      <c r="AM8">
         <v>4</v>
       </c>
-      <c r="AM8" t="s">
+      <c r="AO8" t="s">
         <v>124</v>
       </c>
-      <c r="AN8" t="s">
+      <c r="AP8" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:43">
       <c r="A9" t="s">
         <v>125</v>
       </c>
@@ -1907,83 +1970,89 @@
       <c r="N9" t="s">
         <v>133</v>
       </c>
-      <c r="O9" t="s">
+      <c r="O9">
+        <v>13.07</v>
+      </c>
+      <c r="P9">
+        <v>199</v>
+      </c>
+      <c r="Q9" t="s">
         <v>134</v>
       </c>
-      <c r="P9" t="s">
+      <c r="R9" t="s">
         <v>135</v>
       </c>
-      <c r="Q9">
+      <c r="S9">
         <v>202</v>
       </c>
-      <c r="R9">
+      <c r="T9">
         <v>50</v>
       </c>
-      <c r="S9">
+      <c r="U9">
         <v>0.99999990000000005</v>
       </c>
-      <c r="T9">
+      <c r="V9">
         <v>0.93089999999999995</v>
       </c>
-      <c r="U9" t="s">
+      <c r="W9" t="s">
         <v>180</v>
       </c>
-      <c r="V9">
+      <c r="X9">
         <v>53</v>
       </c>
-      <c r="W9">
+      <c r="Y9">
         <v>5</v>
       </c>
-      <c r="X9" s="1">
+      <c r="Z9" s="1">
         <v>0.45</v>
       </c>
-      <c r="Y9" s="1">
+      <c r="AA9" s="1">
         <v>31.5</v>
       </c>
-      <c r="Z9" s="2">
+      <c r="AB9" s="2">
         <v>42424</v>
       </c>
-      <c r="AA9" s="2">
+      <c r="AC9" s="2">
         <v>42436</v>
-      </c>
-      <c r="AB9" s="2">
-        <v>42437</v>
-      </c>
-      <c r="AC9" s="2">
-        <v>42437</v>
       </c>
       <c r="AD9" s="2">
         <v>42437</v>
       </c>
-      <c r="AE9" t="s">
+      <c r="AE9" s="2">
+        <v>42437</v>
+      </c>
+      <c r="AF9" s="2">
+        <v>42437</v>
+      </c>
+      <c r="AG9" t="s">
         <v>136</v>
       </c>
-      <c r="AF9">
-        <v>1</v>
-      </c>
-      <c r="AG9">
+      <c r="AH9">
+        <v>1</v>
+      </c>
+      <c r="AI9">
         <v>50</v>
       </c>
-      <c r="AH9" t="s">
+      <c r="AJ9" t="s">
         <v>66</v>
       </c>
-      <c r="AI9">
-        <v>1</v>
-      </c>
-      <c r="AJ9">
-        <v>1</v>
-      </c>
       <c r="AK9">
+        <v>1</v>
+      </c>
+      <c r="AL9">
+        <v>1</v>
+      </c>
+      <c r="AM9">
         <v>6</v>
       </c>
-      <c r="AM9" t="s">
+      <c r="AO9" t="s">
         <v>137</v>
       </c>
-      <c r="AN9" t="s">
+      <c r="AP9" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:43">
       <c r="A10" t="s">
         <v>138</v>
       </c>
@@ -2026,83 +2095,90 @@
       <c r="N10" t="s">
         <v>86</v>
       </c>
-      <c r="O10" t="s">
+      <c r="O10">
+        <f>SQRT(75.02)</f>
+        <v>8.6614086614129917</v>
+      </c>
+      <c r="P10">
+        <v>78</v>
+      </c>
+      <c r="Q10" t="s">
         <v>145</v>
       </c>
-      <c r="P10" t="s">
+      <c r="R10" t="s">
         <v>146</v>
       </c>
-      <c r="Q10">
+      <c r="S10">
         <v>80</v>
       </c>
-      <c r="R10">
+      <c r="T10">
         <v>80</v>
       </c>
-      <c r="S10">
+      <c r="U10">
         <v>0.88</v>
       </c>
-      <c r="T10">
+      <c r="V10">
         <v>0.8</v>
       </c>
-      <c r="U10" t="s">
+      <c r="W10" t="s">
         <v>64</v>
       </c>
-      <c r="V10">
+      <c r="X10">
         <v>84</v>
       </c>
-      <c r="W10">
+      <c r="Y10">
         <v>10</v>
       </c>
-      <c r="X10" s="1">
+      <c r="Z10" s="1">
         <v>0.9</v>
       </c>
-      <c r="Y10" s="1">
+      <c r="AA10" s="1">
         <v>100.8</v>
       </c>
-      <c r="Z10" s="2">
+      <c r="AB10" s="2">
         <v>42418</v>
       </c>
-      <c r="AA10" s="2">
+      <c r="AC10" s="2">
         <v>42430</v>
       </c>
-      <c r="AB10" s="2">
+      <c r="AD10" s="2">
         <v>42435</v>
       </c>
-      <c r="AC10" s="2">
+      <c r="AE10" s="2">
         <v>42435</v>
       </c>
-      <c r="AD10" s="2">
+      <c r="AF10" s="2">
         <v>42437</v>
       </c>
-      <c r="AE10" t="s">
+      <c r="AG10" t="s">
         <v>147</v>
       </c>
-      <c r="AF10">
-        <v>1</v>
-      </c>
-      <c r="AG10">
+      <c r="AH10">
+        <v>1</v>
+      </c>
+      <c r="AI10">
         <v>84</v>
       </c>
-      <c r="AH10" t="s">
+      <c r="AJ10" t="s">
         <v>148</v>
       </c>
-      <c r="AI10">
-        <v>1</v>
-      </c>
-      <c r="AJ10">
-        <v>1</v>
-      </c>
       <c r="AK10">
+        <v>1</v>
+      </c>
+      <c r="AL10">
+        <v>1</v>
+      </c>
+      <c r="AM10">
         <v>6.5</v>
       </c>
-      <c r="AM10" t="s">
+      <c r="AO10" t="s">
         <v>149</v>
       </c>
-      <c r="AN10" t="s">
+      <c r="AP10" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:43">
       <c r="A11" t="s">
         <v>150</v>
       </c>
@@ -2139,83 +2215,90 @@
       <c r="N11">
         <v>0.04</v>
       </c>
-      <c r="O11" t="s">
+      <c r="O11">
+        <f>SQRT(4.08)</f>
+        <v>2.0199009876724157</v>
+      </c>
+      <c r="P11">
+        <v>309</v>
+      </c>
+      <c r="Q11" t="s">
         <v>157</v>
       </c>
-      <c r="P11">
-        <v>0.36</v>
-      </c>
-      <c r="Q11">
+      <c r="R11" t="s">
+        <v>181</v>
+      </c>
+      <c r="S11">
         <v>312</v>
       </c>
-      <c r="R11">
+      <c r="T11">
         <v>312</v>
       </c>
-      <c r="S11">
+      <c r="U11">
         <v>0.52</v>
       </c>
-      <c r="T11">
+      <c r="V11">
         <v>0.88</v>
       </c>
-      <c r="U11" t="s">
+      <c r="W11" t="s">
         <v>51</v>
       </c>
-      <c r="V11">
+      <c r="X11">
         <v>328</v>
       </c>
-      <c r="W11" s="3">
+      <c r="Y11" s="3">
         <v>42406</v>
       </c>
-      <c r="X11" s="1">
+      <c r="Z11" s="1">
         <v>0.4</v>
       </c>
-      <c r="Y11" s="1">
+      <c r="AA11" s="1">
         <v>174.72</v>
       </c>
-      <c r="Z11" s="2">
+      <c r="AB11" s="2">
         <v>42418</v>
-      </c>
-      <c r="AA11" s="2">
-        <v>42437</v>
-      </c>
-      <c r="AB11" s="2">
-        <v>42437</v>
       </c>
       <c r="AC11" s="2">
         <v>42437</v>
       </c>
       <c r="AD11" s="2">
+        <v>42437</v>
+      </c>
+      <c r="AE11" s="2">
+        <v>42437</v>
+      </c>
+      <c r="AF11" s="2">
         <v>42438</v>
       </c>
-      <c r="AE11" t="s">
+      <c r="AG11" t="s">
         <v>158</v>
       </c>
-      <c r="AF11">
-        <v>1</v>
-      </c>
-      <c r="AG11">
+      <c r="AH11">
+        <v>1</v>
+      </c>
+      <c r="AI11">
         <v>328</v>
       </c>
-      <c r="AH11" t="s">
+      <c r="AJ11" t="s">
         <v>66</v>
       </c>
-      <c r="AI11">
+      <c r="AK11">
         <v>0.5</v>
       </c>
-      <c r="AJ11">
+      <c r="AL11">
         <v>0.5</v>
       </c>
-      <c r="AK11">
+      <c r="AM11">
         <v>4.5</v>
       </c>
-      <c r="AM11" t="s">
+      <c r="AO11" t="s">
         <v>159</v>
       </c>
-      <c r="AN11" t="s">
+      <c r="AP11" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:43">
       <c r="A12" t="s">
         <v>160</v>
       </c>
@@ -2258,92 +2341,104 @@
       <c r="N12">
         <v>1E-3</v>
       </c>
-      <c r="O12" t="s">
+      <c r="O12">
+        <f>SQRT(32.04)</f>
+        <v>5.6603886792339626</v>
+      </c>
+      <c r="P12">
+        <v>11</v>
+      </c>
+      <c r="Q12" t="s">
         <v>167</v>
       </c>
-      <c r="P12" t="s">
+      <c r="R12" t="s">
         <v>168</v>
       </c>
-      <c r="Q12">
+      <c r="S12">
         <v>12</v>
       </c>
-      <c r="R12">
+      <c r="T12">
         <v>12</v>
       </c>
-      <c r="S12">
+      <c r="U12">
         <v>0.92</v>
       </c>
-      <c r="T12">
+      <c r="V12">
         <v>0.92</v>
       </c>
-      <c r="U12" t="s">
+      <c r="W12" t="s">
         <v>51</v>
       </c>
-      <c r="V12">
+      <c r="X12">
         <v>13</v>
       </c>
-      <c r="W12">
+      <c r="Y12">
         <v>60</v>
       </c>
-      <c r="X12" s="1">
+      <c r="Z12" s="1">
         <v>5</v>
       </c>
-      <c r="Y12" s="1">
+      <c r="AA12" s="1">
         <v>84</v>
       </c>
-      <c r="Z12" s="2">
+      <c r="AB12" s="2">
         <v>42419</v>
       </c>
-      <c r="AA12" s="2">
+      <c r="AC12" s="2">
         <v>42434</v>
       </c>
-      <c r="AB12" s="2">
+      <c r="AD12" s="2">
         <v>42436</v>
       </c>
-      <c r="AC12" s="2">
+      <c r="AE12" s="2">
         <v>42438</v>
       </c>
-      <c r="AD12" s="2">
+      <c r="AF12" s="2">
         <v>42438</v>
       </c>
-      <c r="AE12" t="s">
+      <c r="AG12" t="s">
         <v>169</v>
       </c>
-      <c r="AF12">
-        <v>1</v>
-      </c>
-      <c r="AG12">
+      <c r="AH12">
+        <v>1</v>
+      </c>
+      <c r="AI12">
         <v>27</v>
       </c>
-      <c r="AH12" t="s">
+      <c r="AJ12" t="s">
         <v>53</v>
       </c>
-      <c r="AI12">
+      <c r="AK12">
         <v>0.5</v>
       </c>
-      <c r="AJ12">
+      <c r="AL12">
         <v>0</v>
       </c>
-      <c r="AK12">
+      <c r="AM12">
         <v>4</v>
       </c>
-      <c r="AM12" t="s">
+      <c r="AO12" t="s">
         <v>170</v>
       </c>
-      <c r="AN12" t="s">
+      <c r="AP12" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="X16" s="1"/>
-      <c r="Y16" s="1"/>
-      <c r="Z16" s="2"/>
-      <c r="AA16" s="2"/>
+    <row r="16" spans="1:43">
+      <c r="Z16" s="1"/>
+      <c r="AA16" s="1"/>
       <c r="AB16" s="2"/>
       <c r="AC16" s="2"/>
       <c r="AD16" s="2"/>
+      <c r="AE16" s="2"/>
+      <c r="AF16" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed excel binary merge
</commit_message>
<xml_diff>
--- a/data/planning_and_outcomes.xlsx
+++ b/data/planning_and_outcomes.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="182">
   <si>
     <t>project_key</t>
   </si>
@@ -171,9 +171,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>F-test (2x2 ANOVA)</t>
-  </si>
-  <si>
     <t>F(1,46)=7.89</t>
   </si>
   <si>
@@ -420,12 +417,6 @@
     <t>1b</t>
   </si>
   <si>
-    <t>t-test (regression)</t>
-  </si>
-  <si>
-    <t>&lt; .001</t>
-  </si>
-  <si>
     <t>t(199) = 13.07</t>
   </si>
   <si>
@@ -456,9 +447,6 @@
     <t>Gender Bias in Attributing Creativity</t>
   </si>
   <si>
-    <t>Mixed-Model ANOVA</t>
-  </si>
-  <si>
     <t>F(1,78)=75.02,p&lt;.001</t>
   </si>
   <si>
@@ -492,9 +480,6 @@
     <t>How Will I Be Remembered?</t>
   </si>
   <si>
-    <t>F test (regression)</t>
-  </si>
-  <si>
     <t>F(1, 309)=4.08</t>
   </si>
   <si>
@@ -522,9 +507,6 @@
     <t>Capacity for Visual Features in Mental Rotation</t>
   </si>
   <si>
-    <t>F test (ANOVA within subjects)</t>
-  </si>
-  <si>
     <t>F(1,11)=32.04</t>
   </si>
   <si>
@@ -537,6 +519,9 @@
     <t>http://rpubs.com/lampinen/155174</t>
   </si>
   <si>
+    <t>&lt;0.001</t>
+  </si>
+  <si>
     <t>interaction</t>
   </si>
   <si>
@@ -561,13 +546,19 @@
     <t>d = .51</t>
   </si>
   <si>
-    <t>&lt; 0.001</t>
-  </si>
-  <si>
     <t>Conservative</t>
   </si>
   <si>
-    <t>d=0.36</t>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>power analysis incorrect, DFT x condition interaction is key test</t>
+  </si>
+  <si>
+    <t>effect chosen is more of a manipulation check, individual cue effects (six in all) were the focus of the study, more descriptive</t>
+  </si>
+  <si>
+    <t>chose a main effect but actually the interaction was more theoretically significant, and actually replicated</t>
   </si>
   <si>
     <t>original_t_stat</t>
@@ -621,14 +612,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -906,19 +898,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ16"/>
+  <dimension ref="A1:AR16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P13" sqref="P13"/>
+      <selection pane="bottomLeft" activeCell="AP15" sqref="AP15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="16" max="16" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43">
+    <row r="1" spans="1:44">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -959,13 +952,13 @@
         <v>12</v>
       </c>
       <c r="N1" t="s">
+        <v>179</v>
+      </c>
+      <c r="O1" t="s">
+        <v>180</v>
+      </c>
+      <c r="P1" t="s">
         <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>182</v>
-      </c>
-      <c r="P1" t="s">
-        <v>183</v>
       </c>
       <c r="Q1" t="s">
         <v>14</v>
@@ -1037,7 +1030,7 @@
         <v>36</v>
       </c>
       <c r="AN1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="AO1" t="s">
         <v>37</v>
@@ -1048,8 +1041,11 @@
       <c r="AQ1" t="s">
         <v>39</v>
       </c>
+      <c r="AR1" t="s">
+        <v>175</v>
+      </c>
     </row>
-    <row r="2" spans="1:43">
+    <row r="2" spans="1:44">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -1077,33 +1073,33 @@
       <c r="I2" t="s">
         <v>46</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="4" t="s">
         <v>48</v>
       </c>
       <c r="L2" t="s">
         <v>46</v>
       </c>
       <c r="M2" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="N2">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="O2">
         <f>SQRT(7.89)</f>
         <v>2.8089143810376278</v>
       </c>
+      <c r="O2">
+        <v>46</v>
+      </c>
       <c r="P2">
-        <v>46</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="Q2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="R2" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="S2">
         <v>48</v>
@@ -1118,7 +1114,7 @@
         <v>0.82</v>
       </c>
       <c r="W2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="X2">
         <v>51</v>
@@ -1148,7 +1144,7 @@
         <v>42441</v>
       </c>
       <c r="AG2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AH2">
         <v>1</v>
@@ -1157,7 +1153,7 @@
         <v>61</v>
       </c>
       <c r="AJ2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AK2">
         <v>0.5</v>
@@ -1172,33 +1168,33 @@
         <v>1</v>
       </c>
       <c r="AO2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP2" t="s">
         <v>54</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AQ2" t="s">
         <v>55</v>
       </c>
-      <c r="AQ2" t="s">
+    </row>
+    <row r="3" spans="1:44">
+      <c r="A3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="3" spans="1:43">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>57</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>58</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>59</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>60</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>61</v>
-      </c>
-      <c r="F3" t="s">
-        <v>62</v>
       </c>
       <c r="G3">
         <v>4</v>
@@ -1219,23 +1215,23 @@
         <v>48</v>
       </c>
       <c r="M3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="N3">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="O3">
         <f>SQRT(7.497)</f>
         <v>2.7380650101851125</v>
       </c>
+      <c r="O3">
+        <v>115</v>
+      </c>
       <c r="P3">
-        <v>115</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="Q3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R3" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="S3">
         <v>122</v>
@@ -1250,7 +1246,7 @@
         <v>0.8</v>
       </c>
       <c r="W3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="X3">
         <v>130</v>
@@ -1280,7 +1276,7 @@
         <v>42441</v>
       </c>
       <c r="AG3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AH3">
         <v>1</v>
@@ -1289,7 +1285,7 @@
         <v>128</v>
       </c>
       <c r="AJ3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AK3">
         <v>0.5</v>
@@ -1304,33 +1300,33 @@
         <v>1</v>
       </c>
       <c r="AO3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="AP3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ3" t="s">
         <v>55</v>
       </c>
-      <c r="AQ3" t="s">
-        <v>56</v>
-      </c>
     </row>
-    <row r="4" spans="1:43">
+    <row r="4" spans="1:44">
       <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" t="s">
         <v>67</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>68</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>69</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>70</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>71</v>
-      </c>
-      <c r="F4" t="s">
-        <v>72</v>
       </c>
       <c r="G4">
         <v>3</v>
@@ -1345,23 +1341,23 @@
         <v>48</v>
       </c>
       <c r="M4" t="s">
-        <v>171</v>
-      </c>
-      <c r="N4" t="s">
-        <v>73</v>
-      </c>
-      <c r="O4">
+        <v>166</v>
+      </c>
+      <c r="N4">
         <f>2.42</f>
         <v>2.42</v>
       </c>
-      <c r="P4">
+      <c r="O4">
         <v>257</v>
       </c>
+      <c r="P4" t="s">
+        <v>72</v>
+      </c>
       <c r="Q4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="R4" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="S4">
         <v>550</v>
@@ -1376,7 +1372,7 @@
         <v>0.8</v>
       </c>
       <c r="W4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="X4">
         <v>124</v>
@@ -1399,12 +1395,12 @@
       <c r="AD4" s="2">
         <v>42508</v>
       </c>
-      <c r="AE4" s="6"/>
+      <c r="AE4" s="5"/>
       <c r="AF4" s="2">
         <v>42520</v>
       </c>
       <c r="AG4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AH4">
         <v>1</v>
@@ -1413,7 +1409,7 @@
         <v>124</v>
       </c>
       <c r="AJ4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AK4">
         <v>0</v>
@@ -1428,36 +1424,36 @@
         <v>1</v>
       </c>
       <c r="AO4" t="s">
+        <v>76</v>
+      </c>
+      <c r="AP4" t="s">
         <v>77</v>
       </c>
-      <c r="AP4" t="s">
+    </row>
+    <row r="5" spans="1:44">
+      <c r="A5" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="5" spans="1:43">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>79</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>80</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>81</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>82</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>83</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
         <v>84</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5" t="s">
-        <v>85</v>
       </c>
       <c r="I5" t="s">
         <v>46</v>
@@ -1466,22 +1462,22 @@
         <v>46</v>
       </c>
       <c r="M5" t="s">
-        <v>174</v>
-      </c>
-      <c r="N5" t="s">
+        <v>169</v>
+      </c>
+      <c r="N5">
+        <v>5.22</v>
+      </c>
+      <c r="O5">
+        <v>17</v>
+      </c>
+      <c r="P5" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q5" t="s">
         <v>86</v>
       </c>
-      <c r="O5">
-        <v>5.22</v>
-      </c>
-      <c r="P5">
-        <v>17</v>
-      </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>87</v>
-      </c>
-      <c r="R5" t="s">
-        <v>88</v>
       </c>
       <c r="S5">
         <v>18</v>
@@ -1496,7 +1492,7 @@
         <v>0.95499999999999996</v>
       </c>
       <c r="W5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="X5">
         <v>19</v>
@@ -1526,16 +1522,16 @@
         <v>42445</v>
       </c>
       <c r="AG5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AH5">
         <v>1</v>
       </c>
-      <c r="AI5" s="4">
+      <c r="AI5" s="3">
         <v>19</v>
       </c>
       <c r="AJ5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AK5">
         <v>0.5</v>
@@ -1550,30 +1546,30 @@
         <v>1</v>
       </c>
       <c r="AO5" t="s">
+        <v>89</v>
+      </c>
+      <c r="AP5" t="s">
         <v>90</v>
       </c>
-      <c r="AP5" t="s">
-        <v>91</v>
-      </c>
     </row>
-    <row r="6" spans="1:43">
+    <row r="6" spans="1:44">
       <c r="A6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" t="s">
         <v>93</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>94</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>95</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>96</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>97</v>
-      </c>
-      <c r="F6" t="s">
-        <v>98</v>
       </c>
       <c r="G6">
         <v>2</v>
@@ -1594,23 +1590,23 @@
         <v>46</v>
       </c>
       <c r="M6" t="s">
-        <v>171</v>
-      </c>
-      <c r="N6" t="s">
-        <v>73</v>
-      </c>
-      <c r="O6">
+        <v>166</v>
+      </c>
+      <c r="N6">
         <f>SQRT(5.18)</f>
         <v>2.2759613353482084</v>
       </c>
-      <c r="P6">
+      <c r="O6">
         <v>209</v>
       </c>
+      <c r="P6" t="s">
+        <v>72</v>
+      </c>
       <c r="Q6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="R6" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="S6">
         <v>219</v>
@@ -1625,7 +1621,7 @@
         <v>0.8</v>
       </c>
       <c r="W6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="X6">
         <v>415</v>
@@ -1655,7 +1651,7 @@
         <v>42445</v>
       </c>
       <c r="AG6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AH6">
         <v>1</v>
@@ -1664,7 +1660,7 @@
         <v>397</v>
       </c>
       <c r="AJ6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AK6">
         <v>0</v>
@@ -1679,30 +1675,30 @@
         <v>1</v>
       </c>
       <c r="AO6" t="s">
+        <v>101</v>
+      </c>
+      <c r="AP6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:44">
+      <c r="A7" t="s">
         <v>102</v>
       </c>
-      <c r="AP6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:43">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>103</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>104</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>105</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>106</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>107</v>
-      </c>
-      <c r="F7" t="s">
-        <v>108</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -1717,22 +1713,22 @@
         <v>46</v>
       </c>
       <c r="M7" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="N7" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="O7" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="P7" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q7" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="R7" s="4" t="s">
         <v>109</v>
-      </c>
-      <c r="R7" s="5" t="s">
-        <v>110</v>
       </c>
       <c r="S7">
         <v>48</v>
@@ -1740,14 +1736,14 @@
       <c r="T7">
         <v>90</v>
       </c>
-      <c r="U7" s="5">
+      <c r="U7" s="4">
         <v>0.57599999999999996</v>
       </c>
       <c r="V7">
         <v>0.8</v>
       </c>
-      <c r="W7" s="5" t="s">
-        <v>180</v>
+      <c r="W7" s="4" t="s">
+        <v>174</v>
       </c>
       <c r="X7">
         <v>95</v>
@@ -1777,7 +1773,7 @@
         <v>42437</v>
       </c>
       <c r="AG7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AH7">
         <v>1</v>
@@ -1786,7 +1782,7 @@
         <v>95</v>
       </c>
       <c r="AJ7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AK7">
         <v>0.5</v>
@@ -1797,40 +1793,43 @@
       <c r="AM7">
         <v>4</v>
       </c>
-      <c r="AN7" s="5">
+      <c r="AN7" s="4">
         <v>0</v>
       </c>
       <c r="AO7" t="s">
+        <v>111</v>
+      </c>
+      <c r="AP7" t="s">
         <v>112</v>
       </c>
-      <c r="AP7" t="s">
+      <c r="AR7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" spans="1:44">
+      <c r="A8" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="8" spans="1:43">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>114</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>115</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>116</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>117</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>118</v>
-      </c>
-      <c r="F8" t="s">
-        <v>119</v>
       </c>
       <c r="G8">
         <v>2</v>
       </c>
       <c r="H8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I8" t="s">
         <v>48</v>
@@ -1845,23 +1844,23 @@
         <v>46</v>
       </c>
       <c r="M8" t="s">
-        <v>49</v>
-      </c>
-      <c r="N8" t="s">
-        <v>86</v>
-      </c>
-      <c r="O8">
+        <v>169</v>
+      </c>
+      <c r="N8">
         <f>SQRT(83.67)</f>
         <v>9.1471306976559603</v>
       </c>
-      <c r="P8">
+      <c r="O8">
         <v>55</v>
       </c>
+      <c r="P8" t="s">
+        <v>85</v>
+      </c>
       <c r="Q8" t="s">
+        <v>119</v>
+      </c>
+      <c r="R8" t="s">
         <v>120</v>
-      </c>
-      <c r="R8" t="s">
-        <v>121</v>
       </c>
       <c r="S8">
         <v>40</v>
@@ -1876,7 +1875,7 @@
         <v>0.95</v>
       </c>
       <c r="W8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="X8">
         <v>42</v>
@@ -1906,7 +1905,7 @@
         <v>42441</v>
       </c>
       <c r="AG8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AH8">
         <v>1</v>
@@ -1915,7 +1914,7 @@
         <v>40</v>
       </c>
       <c r="AJ8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AK8">
         <v>1</v>
@@ -1926,34 +1925,40 @@
       <c r="AM8">
         <v>4</v>
       </c>
+      <c r="AN8" s="4">
+        <v>0</v>
+      </c>
       <c r="AO8" t="s">
+        <v>123</v>
+      </c>
+      <c r="AP8" t="s">
+        <v>77</v>
+      </c>
+      <c r="AR8" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="9" spans="1:44">
+      <c r="A9" t="s">
         <v>124</v>
       </c>
-      <c r="AP8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:43">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
         <v>125</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>126</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>127</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>128</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>129</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>130</v>
-      </c>
-      <c r="G9" t="s">
-        <v>131</v>
       </c>
       <c r="H9" t="s">
         <v>48</v>
@@ -1965,22 +1970,22 @@
         <v>48</v>
       </c>
       <c r="M9" t="s">
+        <v>169</v>
+      </c>
+      <c r="N9">
+        <v>13.07</v>
+      </c>
+      <c r="O9">
+        <v>199</v>
+      </c>
+      <c r="P9" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>131</v>
+      </c>
+      <c r="R9" t="s">
         <v>132</v>
-      </c>
-      <c r="N9" t="s">
-        <v>133</v>
-      </c>
-      <c r="O9">
-        <v>13.07</v>
-      </c>
-      <c r="P9">
-        <v>199</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>134</v>
-      </c>
-      <c r="R9" t="s">
-        <v>135</v>
       </c>
       <c r="S9">
         <v>202</v>
@@ -1995,7 +2000,7 @@
         <v>0.93089999999999995</v>
       </c>
       <c r="W9" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="X9">
         <v>53</v>
@@ -2025,7 +2030,7 @@
         <v>42437</v>
       </c>
       <c r="AG9" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AH9">
         <v>1</v>
@@ -2034,7 +2039,7 @@
         <v>50</v>
       </c>
       <c r="AJ9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AK9">
         <v>1</v>
@@ -2045,31 +2050,34 @@
       <c r="AM9">
         <v>6</v>
       </c>
+      <c r="AN9">
+        <v>1</v>
+      </c>
       <c r="AO9" t="s">
+        <v>134</v>
+      </c>
+      <c r="AP9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:44">
+      <c r="A10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10" t="s">
+        <v>136</v>
+      </c>
+      <c r="C10" t="s">
         <v>137</v>
       </c>
-      <c r="AP9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:43">
-      <c r="A10" t="s">
+      <c r="D10" t="s">
         <v>138</v>
       </c>
-      <c r="B10" t="s">
+      <c r="E10" t="s">
         <v>139</v>
       </c>
-      <c r="C10" t="s">
+      <c r="F10" t="s">
         <v>140</v>
-      </c>
-      <c r="D10" t="s">
-        <v>141</v>
-      </c>
-      <c r="E10" t="s">
-        <v>142</v>
-      </c>
-      <c r="F10" t="s">
-        <v>143</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -2083,30 +2091,30 @@
       <c r="J10" s="2">
         <v>42775</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="K10" s="4" t="s">
         <v>48</v>
       </c>
       <c r="L10" t="s">
         <v>48</v>
       </c>
-      <c r="M10" t="s">
-        <v>144</v>
-      </c>
-      <c r="N10" t="s">
-        <v>86</v>
-      </c>
-      <c r="O10">
+      <c r="M10" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="N10">
         <f>SQRT(75.02)</f>
         <v>8.6614086614129917</v>
       </c>
-      <c r="P10">
+      <c r="O10">
         <v>78</v>
       </c>
+      <c r="P10" t="s">
+        <v>85</v>
+      </c>
       <c r="Q10" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="R10" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="S10">
         <v>80</v>
@@ -2121,7 +2129,7 @@
         <v>0.8</v>
       </c>
       <c r="W10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="X10">
         <v>84</v>
@@ -2151,7 +2159,7 @@
         <v>42437</v>
       </c>
       <c r="AG10" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="AH10">
         <v>1</v>
@@ -2160,7 +2168,7 @@
         <v>84</v>
       </c>
       <c r="AJ10" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="AK10">
         <v>1</v>
@@ -2171,31 +2179,37 @@
       <c r="AM10">
         <v>6.5</v>
       </c>
+      <c r="AN10" s="4">
+        <v>0</v>
+      </c>
       <c r="AO10" t="s">
+        <v>145</v>
+      </c>
+      <c r="AP10" t="s">
+        <v>112</v>
+      </c>
+      <c r="AR10" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="11" spans="1:44">
+      <c r="A11" t="s">
+        <v>146</v>
+      </c>
+      <c r="B11" t="s">
+        <v>147</v>
+      </c>
+      <c r="C11" t="s">
+        <v>148</v>
+      </c>
+      <c r="D11" t="s">
         <v>149</v>
       </c>
-      <c r="AP10" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="11" spans="1:43">
-      <c r="A11" t="s">
+      <c r="E11" t="s">
         <v>150</v>
       </c>
-      <c r="B11" t="s">
+      <c r="F11" t="s">
         <v>151</v>
-      </c>
-      <c r="C11" t="s">
-        <v>152</v>
-      </c>
-      <c r="D11" t="s">
-        <v>153</v>
-      </c>
-      <c r="E11" t="s">
-        <v>154</v>
-      </c>
-      <c r="F11" t="s">
-        <v>155</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -2210,23 +2224,23 @@
         <v>48</v>
       </c>
       <c r="M11" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="N11">
-        <v>0.04</v>
-      </c>
-      <c r="O11">
         <f>SQRT(4.08)</f>
         <v>2.0199009876724157</v>
       </c>
+      <c r="O11">
+        <v>309</v>
+      </c>
       <c r="P11">
-        <v>309</v>
+        <v>0.04</v>
       </c>
       <c r="Q11" t="s">
-        <v>157</v>
-      </c>
-      <c r="R11" t="s">
-        <v>181</v>
+        <v>152</v>
+      </c>
+      <c r="R11">
+        <v>0.36</v>
       </c>
       <c r="S11">
         <v>312</v>
@@ -2241,13 +2255,13 @@
         <v>0.88</v>
       </c>
       <c r="W11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="X11">
         <v>328</v>
       </c>
       <c r="Y11" s="3">
-        <v>42406</v>
+        <v>4</v>
       </c>
       <c r="Z11" s="1">
         <v>0.4</v>
@@ -2271,7 +2285,7 @@
         <v>42438</v>
       </c>
       <c r="AG11" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="AH11">
         <v>1</v>
@@ -2280,7 +2294,7 @@
         <v>328</v>
       </c>
       <c r="AJ11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AK11">
         <v>0.5</v>
@@ -2291,34 +2305,37 @@
       <c r="AM11">
         <v>4.5</v>
       </c>
+      <c r="AN11" s="6">
+        <v>1</v>
+      </c>
       <c r="AO11" t="s">
+        <v>154</v>
+      </c>
+      <c r="AP11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:44">
+      <c r="A12" t="s">
+        <v>155</v>
+      </c>
+      <c r="B12" t="s">
+        <v>156</v>
+      </c>
+      <c r="C12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D12" t="s">
+        <v>158</v>
+      </c>
+      <c r="E12" t="s">
         <v>159</v>
       </c>
-      <c r="AP11" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="12" spans="1:43">
-      <c r="A12" t="s">
+      <c r="F12" t="s">
         <v>160</v>
       </c>
-      <c r="B12" t="s">
-        <v>161</v>
-      </c>
-      <c r="C12" t="s">
-        <v>162</v>
-      </c>
-      <c r="D12" t="s">
-        <v>163</v>
-      </c>
-      <c r="E12" t="s">
-        <v>164</v>
-      </c>
-      <c r="F12" t="s">
-        <v>165</v>
-      </c>
       <c r="G12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H12" t="s">
         <v>46</v>
@@ -2336,23 +2353,23 @@
         <v>46</v>
       </c>
       <c r="M12" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="N12">
-        <v>1E-3</v>
-      </c>
-      <c r="O12">
         <f>SQRT(32.04)</f>
         <v>5.6603886792339626</v>
       </c>
-      <c r="P12">
+      <c r="O12">
         <v>11</v>
       </c>
+      <c r="P12" t="s">
+        <v>165</v>
+      </c>
       <c r="Q12" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="R12" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="S12">
         <v>12</v>
@@ -2367,7 +2384,7 @@
         <v>0.92</v>
       </c>
       <c r="W12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="X12">
         <v>13</v>
@@ -2397,7 +2414,7 @@
         <v>42438</v>
       </c>
       <c r="AG12" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="AH12">
         <v>1</v>
@@ -2406,7 +2423,7 @@
         <v>27</v>
       </c>
       <c r="AJ12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AK12">
         <v>0.5</v>
@@ -2417,14 +2434,17 @@
       <c r="AM12">
         <v>4</v>
       </c>
+      <c r="AN12" s="7">
+        <v>1</v>
+      </c>
       <c r="AO12" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="AP12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:43">
+    <row r="16" spans="1:44">
       <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
       <c r="AB16" s="2"/>

</xml_diff>

<commit_message>
Remove empty rows in csv
</commit_message>
<xml_diff>
--- a/data/planning_and_outcomes.xlsx
+++ b/data/planning_and_outcomes.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="planning_and_outcomes" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -890,7 +890,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -898,11 +898,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR16"/>
+  <dimension ref="A1:AR12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AP15" sqref="AP15"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2444,15 +2444,6 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:44">
-      <c r="Z16" s="1"/>
-      <c r="AA16" s="1"/>
-      <c r="AB16" s="2"/>
-      <c r="AC16" s="2"/>
-      <c r="AD16" s="2"/>
-      <c r="AE16" s="2"/>
-      <c r="AF16" s="2"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>